<commit_message>
new url change and message change
</commit_message>
<xml_diff>
--- a/utility/test.xlsx
+++ b/utility/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SusmitSurwade\IdeaProjects\orange_hrms_trial_app\utility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3BEEEE-79D4-41C7-8F10-C22F59BFA4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F98DC18-741C-4B47-9774-6879954267E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -89,7 +89,7 @@
     <t>Belgian</t>
   </si>
   <si>
-    <t>AW@pB1ssA1</t>
+    <t>aH5o@UmNP5</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -440,6 +440,7 @@
     <col min="1" max="1" width="14.81640625" customWidth="1"/>
     <col min="5" max="5" width="12.36328125" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.08984375" customWidth="1"/>
+    <col min="7" max="7" width="17.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">

</xml_diff>